<commit_message>
Fix: Better column name rules, stop conflicting with opened word or excel file because of the temporary files, number now are rounded to 2 decimal places
</commit_message>
<xml_diff>
--- a/Template Excel.xlsx
+++ b/Template Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joaofrancisco\projetos\generate_word_template_from_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0F44DA-10D7-4B17-A013-12D16E58090E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EEC3A2-3064-4671-9E73-95A33A192444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3540" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>name</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>this is a text template from joao</t>
+  </si>
+  <si>
+    <t>Template_rules_1</t>
+  </si>
+  <si>
+    <t>Do not use number in the beginning of the column name</t>
+  </si>
+  <si>
+    <t>Do not use special characters in the column name</t>
+  </si>
+  <si>
+    <t>Do not use space bar in column name, use "_" to separate</t>
   </si>
 </sst>
 </file>
@@ -101,12 +113,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{131F1016-44F3-492D-9BA5-94405677E2AE}" name="Tabela1" displayName="Tabela1" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{131F1016-44F3-492D-9BA5-94405677E2AE}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{131F1016-44F3-492D-9BA5-94405677E2AE}" name="Tabela1" displayName="Tabela1" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{131F1016-44F3-492D-9BA5-94405677E2AE}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7B84490C-BBAF-40FA-9EB6-2532115B7682}" name="name"/>
     <tableColumn id="2" xr3:uid="{AA75C49F-B91B-45FE-AF00-98427B0D606D}" name="age"/>
     <tableColumn id="3" xr3:uid="{695D1C75-F424-4E5D-B2AE-EF0EC8E7B15F}" name="text"/>
+    <tableColumn id="4" xr3:uid="{7829CAA8-0AF6-4F19-A4DA-71E6C976D5F9}" name="Template_rules_1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -375,7 +388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -385,9 +398,10 @@
   <cols>
     <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,8 +411,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -408,8 +425,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -418,6 +438,14 @@
       </c>
       <c r="C3" t="s">
         <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>